<commit_message>
Fixed typos in column names Babylab_westernSydney #6
</commit_message>
<xml_diff>
--- a/processed_data/handcoded_cleaned/Babylab_WesternSydney_12-15m_bi_GF_Trial.xlsx
+++ b/processed_data/handcoded_cleaned/Babylab_WesternSydney_12-15m_bi_GF_Trial.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21301"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2FBCDE92-1AA8-4F18-B55B-F544A21B2019}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="10515" windowHeight="5190" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="40" windowWidth="25780" windowHeight="15700" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -53,9 +55,6 @@
   </si>
   <si>
     <t>fixation_congruent</t>
-  </si>
-  <si>
-    <t>fixation_incongrent</t>
   </si>
   <si>
     <t>trial_error</t>
@@ -162,12 +161,15 @@
   <si>
     <t>fussy baby</t>
   </si>
+  <si>
+    <t>fixation_incongruent</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -266,7 +268,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -318,7 +320,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -543,21 +545,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
-    <col min="10" max="11" width="9.140625" style="4"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="4"/>
+    <col min="10" max="11" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:14" ht="42">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,21 +591,21 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>8285</v>
@@ -612,13 +614,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>15</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
       </c>
       <c r="G2" s="4">
         <v>3.2570000000000001</v>
@@ -636,15 +638,15 @@
         <v>0.98</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>8285</v>
@@ -653,13 +655,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
         <v>19</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
       </c>
       <c r="G3" s="4">
         <v>1.6379999999999999</v>
@@ -677,15 +679,15 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>8285</v>
@@ -694,13 +696,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="4">
         <v>2.246</v>
@@ -718,15 +720,15 @@
         <v>0.442</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>8285</v>
@@ -735,13 +737,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="4">
         <v>2.149</v>
@@ -759,15 +761,15 @@
         <v>0.44900000000000001</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>8285</v>
@@ -776,13 +778,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="4">
         <v>1.9370000000000001</v>
@@ -800,15 +802,15 @@
         <v>1.302</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>8285</v>
@@ -817,13 +819,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G7" s="4">
         <v>4.0119999999999996</v>
@@ -841,15 +843,15 @@
         <v>0.755</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <v>8741</v>
@@ -858,13 +860,13 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="4">
         <v>1.454</v>
@@ -882,15 +884,15 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9">
         <v>8741</v>
@@ -899,13 +901,13 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G9" s="4">
         <v>2.077</v>
@@ -923,15 +925,15 @@
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>8741</v>
@@ -940,13 +942,13 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="4">
         <v>0</v>
@@ -964,15 +966,15 @@
         <v>3.01</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>8741</v>
@@ -981,16 +983,16 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1005,15 +1007,15 @@
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>8741</v>
@@ -1022,13 +1024,13 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4">
         <v>2.1160000000000001</v>
@@ -1046,15 +1048,15 @@
         <v>1.321</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>8741</v>
@@ -1063,13 +1065,13 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G13" s="4">
         <v>1.722</v>
@@ -1087,15 +1089,15 @@
         <v>0</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>8521</v>
@@ -1104,13 +1106,13 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G14" s="4">
         <v>2.6139999999999999</v>
@@ -1128,15 +1130,15 @@
         <v>2.359</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>8521</v>
@@ -1145,13 +1147,13 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G15" s="4">
         <v>2.0609999999999999</v>
@@ -1169,15 +1171,15 @@
         <v>0</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>8521</v>
@@ -1186,13 +1188,13 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G16" s="4">
         <v>3.153</v>
@@ -1210,15 +1212,15 @@
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>8521</v>
@@ -1227,13 +1229,13 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G17" s="4">
         <v>4.1369999999999996</v>
@@ -1251,15 +1253,15 @@
         <v>1.663</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>8521</v>
@@ -1268,16 +1270,16 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1289,15 +1291,15 @@
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19">
         <v>8521</v>
@@ -1306,13 +1308,13 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G19" s="4">
         <v>1.7769999999999999</v>
@@ -1330,15 +1332,15 @@
         <v>1.972</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20">
         <v>8824</v>
@@ -1347,13 +1349,13 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G20" s="4">
         <v>1.528</v>
@@ -1371,15 +1373,15 @@
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>8824</v>
@@ -1388,13 +1390,13 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G21" s="4">
         <v>4.8520000000000003</v>
@@ -1412,15 +1414,15 @@
         <v>0.65</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22">
         <v>8824</v>
@@ -1429,13 +1431,13 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G22" s="4">
         <v>2.5339999999999998</v>
@@ -1453,15 +1455,15 @@
         <v>0.41099999999999998</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23">
         <v>8824</v>
@@ -1470,13 +1472,13 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23">
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G23" s="4">
         <v>1.6619999999999999</v>
@@ -1494,15 +1496,15 @@
         <v>0.85699999999999998</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24">
         <v>8824</v>
@@ -1511,13 +1513,13 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G24" s="4">
         <v>2.2549999999999999</v>
@@ -1535,15 +1537,15 @@
         <v>2.5640000000000001</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B25">
         <v>8824</v>
@@ -1552,13 +1554,13 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G25" s="4">
         <v>3.0390000000000001</v>
@@ -1576,15 +1578,15 @@
         <v>0</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>1171</v>
@@ -1593,16 +1595,16 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1617,15 +1619,15 @@
         <v>0</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27">
         <v>1171</v>
@@ -1634,13 +1636,13 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G27" s="4">
         <v>2.278</v>
@@ -1658,15 +1660,15 @@
         <v>2.0169999999999999</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B28">
         <v>1171</v>
@@ -1675,13 +1677,13 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G28" s="4">
         <v>0</v>
@@ -1699,15 +1701,15 @@
         <v>2.2959999999999998</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B29">
         <v>1171</v>
@@ -1716,13 +1718,13 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G29" s="4">
         <v>0</v>
@@ -1740,15 +1742,15 @@
         <v>0</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30">
         <v>1171</v>
@@ -1757,13 +1759,13 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30">
         <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G30" s="4">
         <v>2.4140000000000001</v>
@@ -1781,15 +1783,15 @@
         <v>0</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B31">
         <v>1171</v>
@@ -1798,13 +1800,13 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31">
         <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G31" s="4">
         <v>3.8820000000000001</v>
@@ -1822,15 +1824,15 @@
         <v>0</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B32">
         <v>904</v>
@@ -1839,13 +1841,13 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G32" s="4">
         <v>2.4079999999999999</v>
@@ -1863,15 +1865,15 @@
         <v>0</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B33">
         <v>904</v>
@@ -1880,16 +1882,16 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E33">
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1904,15 +1906,15 @@
         <v>0</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34">
         <v>904</v>
@@ -1921,13 +1923,13 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E34">
         <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G34" s="4">
         <v>1.758</v>
@@ -1945,15 +1947,15 @@
         <v>1.276</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B35">
         <v>904</v>
@@ -1962,13 +1964,13 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G35" s="4">
         <v>2.0830000000000002</v>
@@ -1986,15 +1988,15 @@
         <v>0</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B36">
         <v>904</v>
@@ -2003,13 +2005,13 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E36">
         <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G36" s="4">
         <v>1.7310000000000001</v>
@@ -2027,15 +2029,15 @@
         <v>0.60499999999999998</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B37">
         <v>904</v>
@@ -2044,13 +2046,13 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E37">
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G37" s="4">
         <v>1.1819999999999999</v>
@@ -2068,15 +2070,15 @@
         <v>0</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B38">
         <v>2140</v>
@@ -2085,16 +2087,16 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2109,15 +2111,15 @@
         <v>0</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B39">
         <v>2140</v>
@@ -2126,13 +2128,13 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G39" s="4">
         <v>1.4179999999999999</v>
@@ -2150,15 +2152,15 @@
         <v>0</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B40">
         <v>2140</v>
@@ -2167,13 +2169,13 @@
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E40">
         <v>3</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G40" s="4">
         <v>2.8250000000000002</v>
@@ -2191,15 +2193,15 @@
         <v>0</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41">
         <v>2140</v>
@@ -2208,16 +2210,16 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E41">
         <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G41" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2232,15 +2234,15 @@
         <v>0</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B42">
         <v>2140</v>
@@ -2249,13 +2251,13 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E42">
         <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G42" s="4">
         <v>3.0579999999999998</v>
@@ -2273,15 +2275,15 @@
         <v>0</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B43">
         <v>2140</v>
@@ -2290,13 +2292,13 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E43">
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G43" s="4">
         <v>1.6659999999999999</v>
@@ -2314,15 +2316,15 @@
         <v>2.6629999999999998</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B44">
         <v>53</v>
@@ -2331,13 +2333,13 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
         <v>15</v>
-      </c>
-      <c r="E44">
-        <v>1</v>
-      </c>
-      <c r="F44" t="s">
-        <v>16</v>
       </c>
       <c r="G44" s="4">
         <v>3.657</v>
@@ -2355,15 +2357,15 @@
         <v>0.44900000000000001</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B45">
         <v>53</v>
@@ -2372,13 +2374,13 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E45">
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G45" s="4">
         <v>3.1970000000000001</v>
@@ -2396,15 +2398,15 @@
         <v>2.5649999999999999</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B46">
         <v>53</v>
@@ -2413,13 +2415,13 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G46" s="4">
         <v>2.5960000000000001</v>
@@ -2437,15 +2439,15 @@
         <v>0</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B47">
         <v>53</v>
@@ -2454,16 +2456,16 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E47">
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2478,15 +2480,15 @@
         <v>0</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B48">
         <v>53</v>
@@ -2495,13 +2497,13 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E48">
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G48" s="4">
         <v>2.044</v>
@@ -2519,15 +2521,15 @@
         <v>0</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B49">
         <v>53</v>
@@ -2536,13 +2538,13 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E49">
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G49" s="4">
         <v>0</v>
@@ -2560,15 +2562,15 @@
         <v>1.1970000000000001</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B50">
         <v>2157</v>
@@ -2577,13 +2579,13 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G50" s="4">
         <v>3.0840000000000001</v>
@@ -2601,15 +2603,15 @@
         <v>1.2569999999999999</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B51">
         <v>2157</v>
@@ -2618,13 +2620,13 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E51">
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G51" s="4">
         <v>2.726</v>
@@ -2642,15 +2644,15 @@
         <v>0</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B52">
         <v>2157</v>
@@ -2659,13 +2661,13 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E52">
         <v>3</v>
       </c>
       <c r="F52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G52" s="4">
         <v>1.44</v>
@@ -2683,15 +2685,15 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B53">
         <v>2157</v>
@@ -2700,13 +2702,13 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E53">
         <v>4</v>
       </c>
       <c r="F53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G53" s="4">
         <v>1.7609999999999999</v>
@@ -2724,15 +2726,15 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54">
         <v>2157</v>
@@ -2741,13 +2743,13 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E54">
         <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G54" s="4">
         <v>1.3540000000000001</v>
@@ -2765,15 +2767,15 @@
         <v>0</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55">
         <v>2157</v>
@@ -2782,13 +2784,13 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E55">
         <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G55" s="4">
         <v>2.8740000000000001</v>
@@ -2806,15 +2808,15 @@
         <v>2.206</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B56">
         <v>2206</v>
@@ -2823,13 +2825,13 @@
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G56" s="4">
         <v>2.5819999999999999</v>
@@ -2847,15 +2849,15 @@
         <v>2.222</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>2206</v>
@@ -2864,13 +2866,13 @@
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E57">
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G57" s="4">
         <v>1.883</v>
@@ -2888,15 +2890,15 @@
         <v>0.85399999999999998</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B58">
         <v>2206</v>
@@ -2905,16 +2907,16 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="F58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G58" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -2929,15 +2931,15 @@
         <v>0</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B59">
         <v>2206</v>
@@ -2946,16 +2948,16 @@
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E59">
         <v>4</v>
       </c>
       <c r="F59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G59" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2970,15 +2972,15 @@
         <v>0</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60">
         <v>2206</v>
@@ -2987,16 +2989,16 @@
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E60">
         <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G60" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3011,15 +3013,15 @@
         <v>0</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B61">
         <v>2206</v>
@@ -3028,13 +3030,13 @@
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E61">
         <v>6</v>
       </c>
       <c r="F61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G61" s="4">
         <v>1.33</v>
@@ -3052,15 +3054,15 @@
         <v>0</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B62">
         <v>2270</v>
@@ -3069,13 +3071,13 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G62" s="4">
         <v>2.202</v>
@@ -3093,15 +3095,15 @@
         <v>0</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B63">
         <v>2270</v>
@@ -3110,13 +3112,13 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63" t="s">
         <v>19</v>
-      </c>
-      <c r="E63">
-        <v>2</v>
-      </c>
-      <c r="F63" t="s">
-        <v>20</v>
       </c>
       <c r="G63" s="4">
         <v>0</v>
@@ -3134,15 +3136,15 @@
         <v>0</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B64">
         <v>2270</v>
@@ -3151,13 +3153,13 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E64">
         <v>3</v>
       </c>
       <c r="F64" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G64" s="4">
         <v>3.9470000000000001</v>
@@ -3175,15 +3177,15 @@
         <v>0</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B65">
         <v>2270</v>
@@ -3192,13 +3194,13 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E65">
         <v>4</v>
       </c>
       <c r="F65" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G65" s="4">
         <v>2.2839999999999998</v>
@@ -3216,15 +3218,15 @@
         <v>1.599</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B66">
         <v>2270</v>
@@ -3233,13 +3235,13 @@
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E66">
         <v>5</v>
       </c>
       <c r="F66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G66" s="4">
         <v>1.42</v>
@@ -3257,15 +3259,15 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B67">
         <v>2270</v>
@@ -3274,13 +3276,13 @@
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E67">
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G67" s="4">
         <v>2.4790000000000001</v>
@@ -3298,15 +3300,15 @@
         <v>1.2649999999999999</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B68">
         <v>2272</v>
@@ -3315,16 +3317,16 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3339,15 +3341,15 @@
         <v>0</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B69">
         <v>2272</v>
@@ -3356,13 +3358,13 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E69">
         <v>2</v>
       </c>
       <c r="F69" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G69" s="4">
         <v>2.5230000000000001</v>
@@ -3380,15 +3382,15 @@
         <v>0</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B70">
         <v>2272</v>
@@ -3397,16 +3399,16 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E70">
         <v>3</v>
       </c>
       <c r="F70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G70" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3421,15 +3423,15 @@
         <v>0</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B71">
         <v>2272</v>
@@ -3438,13 +3440,13 @@
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E71">
         <v>4</v>
       </c>
       <c r="F71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G71" s="4">
         <v>1.137</v>
@@ -3462,15 +3464,15 @@
         <v>0</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B72">
         <v>2272</v>
@@ -3479,16 +3481,16 @@
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E72">
         <v>5</v>
       </c>
       <c r="F72" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3503,15 +3505,15 @@
         <v>0</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B73">
         <v>2272</v>
@@ -3520,13 +3522,13 @@
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E73">
         <v>6</v>
       </c>
       <c r="F73" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G73" s="4">
         <v>2.9860000000000002</v>
@@ -3544,15 +3546,15 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B74">
         <v>2169</v>
@@ -3561,13 +3563,13 @@
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G74" s="4">
         <v>1.696</v>
@@ -3585,15 +3587,15 @@
         <v>0</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B75">
         <v>2169</v>
@@ -3602,13 +3604,13 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E75">
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G75" s="4">
         <v>1.504</v>
@@ -3626,15 +3628,15 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B76">
         <v>2169</v>
@@ -3643,16 +3645,16 @@
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E76">
         <v>3</v>
       </c>
       <c r="F76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3667,15 +3669,15 @@
         <v>0</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B77">
         <v>2169</v>
@@ -3684,16 +3686,16 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E77">
         <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3708,15 +3710,15 @@
         <v>0</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B78">
         <v>2169</v>
@@ -3725,16 +3727,16 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E78">
         <v>5</v>
       </c>
       <c r="F78" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3749,15 +3751,15 @@
         <v>0</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B79">
         <v>2169</v>
@@ -3766,16 +3768,16 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E79">
         <v>6</v>
       </c>
       <c r="F79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -3790,15 +3792,15 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M79" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B80">
         <v>1690</v>
@@ -3807,13 +3809,13 @@
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E80">
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G80" s="4">
         <v>0</v>
@@ -3831,15 +3833,15 @@
         <v>0</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B81">
         <v>1690</v>
@@ -3848,16 +3850,16 @@
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E81">
         <v>2</v>
       </c>
       <c r="F81" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -3872,15 +3874,15 @@
         <v>0</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B82">
         <v>1690</v>
@@ -3889,16 +3891,16 @@
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E82">
         <v>3</v>
       </c>
       <c r="F82" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -3913,15 +3915,15 @@
         <v>0</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B83">
         <v>1690</v>
@@ -3930,16 +3932,16 @@
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E83">
         <v>4</v>
       </c>
       <c r="F83" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -3954,15 +3956,15 @@
         <v>0</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B84">
         <v>1690</v>
@@ -3971,13 +3973,13 @@
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E84">
         <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G84" s="4">
         <v>3.5840000000000001</v>
@@ -3995,15 +3997,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B85">
         <v>1690</v>
@@ -4012,13 +4014,13 @@
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E85">
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G85" s="4">
         <v>1.024</v>
@@ -4036,15 +4038,15 @@
         <v>0</v>
       </c>
       <c r="L85" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M85" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B86">
         <v>716</v>
@@ -4053,13 +4055,13 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E86">
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G86" s="4">
         <v>1.179</v>
@@ -4077,15 +4079,15 @@
         <v>0</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B87">
         <v>716</v>
@@ -4094,13 +4096,13 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E87">
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G87" s="4">
         <v>0.89800000000000002</v>
@@ -4118,15 +4120,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B88">
         <v>716</v>
@@ -4135,13 +4137,13 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E88">
         <v>3</v>
       </c>
       <c r="F88" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G88" s="4">
         <v>1.752</v>
@@ -4159,15 +4161,15 @@
         <v>1.379</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B89">
         <v>716</v>
@@ -4176,13 +4178,13 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E89">
         <v>4</v>
       </c>
       <c r="F89" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G89" s="4">
         <v>3.3029999999999999</v>
@@ -4200,15 +4202,15 @@
         <v>2.375</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B90">
         <v>716</v>
@@ -4217,13 +4219,13 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E90">
         <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G90" s="4">
         <v>1.7190000000000001</v>
@@ -4241,15 +4243,15 @@
         <v>1.028</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B91">
         <v>716</v>
@@ -4258,13 +4260,13 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E91">
         <v>6</v>
       </c>
       <c r="F91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G91" s="4">
         <v>1.7150000000000001</v>
@@ -4282,15 +4284,15 @@
         <v>0</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B92">
         <v>2334</v>
@@ -4299,13 +4301,13 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E92">
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G92" s="4">
         <v>0.91</v>
@@ -4323,15 +4325,15 @@
         <v>0</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B93">
         <v>2334</v>
@@ -4340,16 +4342,16 @@
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E93">
         <v>2</v>
       </c>
       <c r="F93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G93" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -4364,15 +4366,15 @@
         <v>0</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B94">
         <v>2334</v>
@@ -4381,16 +4383,16 @@
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E94">
         <v>3</v>
       </c>
       <c r="F94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G94" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -4405,15 +4407,15 @@
         <v>0</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B95">
         <v>2334</v>
@@ -4422,13 +4424,13 @@
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E95">
         <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G95" s="4">
         <v>1.784</v>
@@ -4446,15 +4448,15 @@
         <v>0</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B96">
         <v>2334</v>
@@ -4463,13 +4465,13 @@
         <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E96">
         <v>5</v>
       </c>
       <c r="F96" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G96" s="4">
         <v>2.133</v>
@@ -4487,15 +4489,15 @@
         <v>0.65700000000000003</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B97">
         <v>2334</v>
@@ -4504,13 +4506,13 @@
         <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E97">
         <v>6</v>
       </c>
       <c r="F97" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G97" s="4">
         <v>0</v>
@@ -4528,15 +4530,15 @@
         <v>0</v>
       </c>
       <c r="L97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M97" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B98" s="2">
         <v>2275</v>
@@ -4545,16 +4547,16 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E98">
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G98" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -4569,15 +4571,15 @@
         <v>0</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B99">
         <v>2275</v>
@@ -4586,13 +4588,13 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E99">
         <v>2</v>
       </c>
       <c r="F99" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G99" s="4">
         <v>3.2989999999999999</v>
@@ -4610,15 +4612,15 @@
         <v>0.71299999999999997</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B100">
         <v>2275</v>
@@ -4627,13 +4629,13 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E100">
         <v>3</v>
       </c>
       <c r="F100" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G100" s="4">
         <v>2.1280000000000001</v>
@@ -4651,15 +4653,15 @@
         <v>0</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B101">
         <v>2275</v>
@@ -4668,16 +4670,16 @@
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E101">
         <v>4</v>
       </c>
       <c r="F101" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G101" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -4692,15 +4694,15 @@
         <v>0</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B102">
         <v>2275</v>
@@ -4709,13 +4711,13 @@
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E102">
         <v>5</v>
       </c>
       <c r="F102" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G102" s="4">
         <v>5.5</v>
@@ -4733,15 +4735,15 @@
         <v>0.316</v>
       </c>
       <c r="L102" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B103">
         <v>2275</v>
@@ -4750,16 +4752,16 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E103">
         <v>6</v>
       </c>
       <c r="F103" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G103" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -4774,10 +4776,10 @@
         <v>0</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -4846,20 +4848,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uploaded corrected files for Babylab_WesternSydney per #41
</commit_message>
<xml_diff>
--- a/processed_data/handcoded_cleaned/Babylab_WesternSydney_12-15m_bi_GF_Trial.xlsx
+++ b/processed_data/handcoded_cleaned/Babylab_WesternSydney_12-15m_bi_GF_Trial.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21421"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32ECD0BA-ACA7-4487-8307-4EF511133549}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="40" windowWidth="25780" windowHeight="15700" firstSheet="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="10515" windowHeight="5190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="12-15m_Bil" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="46">
   <si>
     <t>lab</t>
   </si>
@@ -55,6 +53,9 @@
   </si>
   <si>
     <t>fixation_congruent</t>
+  </si>
+  <si>
+    <t>fixation_incongrent</t>
   </si>
   <si>
     <t>trial_error</t>
@@ -161,15 +162,12 @@
   <si>
     <t>fussy baby</t>
   </si>
-  <si>
-    <t>fixation_incongruent</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -320,7 +318,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -545,21 +543,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="4"/>
-    <col min="10" max="11" width="8.83203125" style="4"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="10" max="11" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="42">
+    <row r="1" spans="1:14" ht="45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,21 +589,21 @@
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>8285</v>
@@ -614,13 +612,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="4">
         <v>3.2570000000000001</v>
@@ -638,15 +636,15 @@
         <v>0.98</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>8285</v>
@@ -655,13 +653,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="4">
         <v>1.6379999999999999</v>
@@ -679,15 +677,15 @@
         <v>0</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>8285</v>
@@ -696,13 +694,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
       </c>
       <c r="G4" s="4">
         <v>2.246</v>
@@ -720,15 +718,15 @@
         <v>0.442</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5">
         <v>8285</v>
@@ -737,13 +735,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="4">
         <v>2.149</v>
@@ -761,15 +759,15 @@
         <v>0.44900000000000001</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>8285</v>
@@ -778,13 +776,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4">
         <v>1.9370000000000001</v>
@@ -802,15 +800,15 @@
         <v>1.302</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>8285</v>
@@ -819,13 +817,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="4">
         <v>4.0119999999999996</v>
@@ -843,15 +841,15 @@
         <v>0.755</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>8741</v>
@@ -860,13 +858,13 @@
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4">
         <v>1.454</v>
@@ -884,15 +882,15 @@
         <v>0</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>8741</v>
@@ -901,13 +899,13 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9" s="4">
         <v>2.077</v>
@@ -925,15 +923,15 @@
         <v>0</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>8741</v>
@@ -942,16 +940,16 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -966,15 +964,15 @@
         <v>3.01</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>8741</v>
@@ -983,16 +981,16 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11">
         <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1007,15 +1005,15 @@
         <v>0</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>8741</v>
@@ -1024,13 +1022,13 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E12">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G12" s="4">
         <v>2.1160000000000001</v>
@@ -1048,15 +1046,15 @@
         <v>1.321</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>8741</v>
@@ -1065,13 +1063,13 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="4">
         <v>1.722</v>
@@ -1089,15 +1087,15 @@
         <v>0</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>8521</v>
@@ -1106,13 +1104,13 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G14" s="4">
         <v>2.6139999999999999</v>
@@ -1130,15 +1128,15 @@
         <v>2.359</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>8521</v>
@@ -1147,13 +1145,13 @@
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G15" s="4">
         <v>2.0609999999999999</v>
@@ -1171,15 +1169,15 @@
         <v>0</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>8521</v>
@@ -1188,13 +1186,13 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>3</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G16" s="4">
         <v>3.153</v>
@@ -1212,15 +1210,15 @@
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B17">
         <v>8521</v>
@@ -1229,13 +1227,13 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E17">
         <v>4</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G17" s="4">
         <v>4.1369999999999996</v>
@@ -1253,15 +1251,15 @@
         <v>1.663</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>8521</v>
@@ -1270,16 +1268,16 @@
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E18">
         <v>5</v>
       </c>
       <c r="F18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1291,15 +1289,15 @@
         <v>0</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>8521</v>
@@ -1308,13 +1306,13 @@
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E19">
         <v>6</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G19" s="4">
         <v>1.7769999999999999</v>
@@ -1332,15 +1330,15 @@
         <v>1.972</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B20">
         <v>8824</v>
@@ -1349,13 +1347,13 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="4">
         <v>1.528</v>
@@ -1373,15 +1371,15 @@
         <v>0</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>8824</v>
@@ -1390,13 +1388,13 @@
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G21" s="4">
         <v>4.8520000000000003</v>
@@ -1414,15 +1412,15 @@
         <v>0.65</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>8824</v>
@@ -1431,13 +1429,13 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E22">
         <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G22" s="4">
         <v>2.5339999999999998</v>
@@ -1455,15 +1453,15 @@
         <v>0.41099999999999998</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>8824</v>
@@ -1472,13 +1470,13 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G23" s="4">
         <v>1.6619999999999999</v>
@@ -1496,15 +1494,15 @@
         <v>0.85699999999999998</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24">
         <v>8824</v>
@@ -1513,13 +1511,13 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E24">
         <v>5</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G24" s="4">
         <v>2.2549999999999999</v>
@@ -1537,15 +1535,15 @@
         <v>2.5640000000000001</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25">
         <v>8824</v>
@@ -1554,13 +1552,13 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E25">
         <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" s="4">
         <v>3.0390000000000001</v>
@@ -1578,15 +1576,15 @@
         <v>0</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26">
         <v>1171</v>
@@ -1595,16 +1593,16 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -1619,15 +1617,15 @@
         <v>0</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B27">
         <v>1171</v>
@@ -1636,13 +1634,13 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G27" s="4">
         <v>2.278</v>
@@ -1660,15 +1658,15 @@
         <v>2.0169999999999999</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28">
         <v>1171</v>
@@ -1677,16 +1675,16 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E28">
         <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="4">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H28">
         <v>1</v>
@@ -1701,15 +1699,15 @@
         <v>2.2959999999999998</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29">
         <v>1171</v>
@@ -1718,16 +1716,16 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H29">
         <v>2</v>
@@ -1742,15 +1740,15 @@
         <v>0</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B30">
         <v>1171</v>
@@ -1759,13 +1757,13 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E30">
         <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G30" s="4">
         <v>2.4140000000000001</v>
@@ -1783,15 +1781,15 @@
         <v>0</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B31">
         <v>1171</v>
@@ -1800,13 +1798,13 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E31">
         <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G31" s="4">
         <v>3.8820000000000001</v>
@@ -1824,15 +1822,15 @@
         <v>0</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B32">
         <v>904</v>
@@ -1841,13 +1839,13 @@
         <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G32" s="4">
         <v>2.4079999999999999</v>
@@ -1865,15 +1863,15 @@
         <v>0</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B33">
         <v>904</v>
@@ -1882,16 +1880,16 @@
         <v>3</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E33">
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -1906,15 +1904,15 @@
         <v>0</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B34">
         <v>904</v>
@@ -1923,13 +1921,13 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E34">
         <v>3</v>
       </c>
       <c r="F34" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G34" s="4">
         <v>1.758</v>
@@ -1947,15 +1945,15 @@
         <v>1.276</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B35">
         <v>904</v>
@@ -1964,13 +1962,13 @@
         <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G35" s="4">
         <v>2.0830000000000002</v>
@@ -1988,15 +1986,15 @@
         <v>0</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B36">
         <v>904</v>
@@ -2005,13 +2003,13 @@
         <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E36">
         <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G36" s="4">
         <v>1.7310000000000001</v>
@@ -2029,15 +2027,15 @@
         <v>0.60499999999999998</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B37">
         <v>904</v>
@@ -2046,13 +2044,13 @@
         <v>3</v>
       </c>
       <c r="D37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E37">
         <v>6</v>
       </c>
       <c r="F37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G37" s="4">
         <v>1.1819999999999999</v>
@@ -2070,15 +2068,15 @@
         <v>0</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:13">
       <c r="A38" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B38">
         <v>2140</v>
@@ -2087,16 +2085,16 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G38" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2111,15 +2109,15 @@
         <v>0</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B39">
         <v>2140</v>
@@ -2128,13 +2126,13 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="F39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G39" s="4">
         <v>1.4179999999999999</v>
@@ -2152,15 +2150,15 @@
         <v>0</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B40">
         <v>2140</v>
@@ -2169,13 +2167,13 @@
         <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E40">
         <v>3</v>
       </c>
       <c r="F40" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G40" s="4">
         <v>2.8250000000000002</v>
@@ -2193,15 +2191,15 @@
         <v>0</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B41">
         <v>2140</v>
@@ -2210,16 +2208,16 @@
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E41">
         <v>4</v>
       </c>
       <c r="F41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G41" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -2234,15 +2232,15 @@
         <v>0</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M41" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B42">
         <v>2140</v>
@@ -2251,13 +2249,13 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E42">
         <v>5</v>
       </c>
       <c r="F42" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G42" s="4">
         <v>3.0579999999999998</v>
@@ -2275,15 +2273,15 @@
         <v>0</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B43">
         <v>2140</v>
@@ -2292,13 +2290,13 @@
         <v>4</v>
       </c>
       <c r="D43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E43">
         <v>6</v>
       </c>
       <c r="F43" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G43" s="4">
         <v>1.6659999999999999</v>
@@ -2316,15 +2314,15 @@
         <v>2.6629999999999998</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M43" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B44">
         <v>53</v>
@@ -2333,13 +2331,13 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G44" s="4">
         <v>3.657</v>
@@ -2357,15 +2355,15 @@
         <v>0.44900000000000001</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B45">
         <v>53</v>
@@ -2374,13 +2372,13 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E45">
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G45" s="4">
         <v>3.1970000000000001</v>
@@ -2398,15 +2396,15 @@
         <v>2.5649999999999999</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B46">
         <v>53</v>
@@ -2415,13 +2413,13 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46" t="s">
         <v>20</v>
-      </c>
-      <c r="E46">
-        <v>3</v>
-      </c>
-      <c r="F46" t="s">
-        <v>19</v>
       </c>
       <c r="G46" s="4">
         <v>2.5960000000000001</v>
@@ -2439,15 +2437,15 @@
         <v>0</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M46" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B47">
         <v>53</v>
@@ -2456,16 +2454,16 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E47">
         <v>4</v>
       </c>
       <c r="F47" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G47" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -2480,15 +2478,15 @@
         <v>0</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B48">
         <v>53</v>
@@ -2497,13 +2495,13 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E48">
         <v>5</v>
       </c>
       <c r="F48" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G48" s="4">
         <v>2.044</v>
@@ -2521,15 +2519,15 @@
         <v>0</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B49">
         <v>53</v>
@@ -2538,16 +2536,16 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E49">
         <v>6</v>
       </c>
       <c r="F49" t="s">
-        <v>43</v>
-      </c>
-      <c r="G49" s="4">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H49">
         <v>1</v>
@@ -2562,15 +2560,15 @@
         <v>1.1970000000000001</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B50">
         <v>2157</v>
@@ -2579,13 +2577,13 @@
         <v>2</v>
       </c>
       <c r="D50" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G50" s="4">
         <v>3.0840000000000001</v>
@@ -2603,15 +2601,15 @@
         <v>1.2569999999999999</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B51">
         <v>2157</v>
@@ -2620,13 +2618,13 @@
         <v>2</v>
       </c>
       <c r="D51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E51">
         <v>2</v>
       </c>
       <c r="F51" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G51" s="4">
         <v>2.726</v>
@@ -2644,15 +2642,15 @@
         <v>0</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B52">
         <v>2157</v>
@@ -2661,13 +2659,13 @@
         <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E52">
         <v>3</v>
       </c>
       <c r="F52" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G52" s="4">
         <v>1.44</v>
@@ -2685,15 +2683,15 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B53">
         <v>2157</v>
@@ -2702,13 +2700,13 @@
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E53">
         <v>4</v>
       </c>
       <c r="F53" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G53" s="4">
         <v>1.7609999999999999</v>
@@ -2726,15 +2724,15 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B54">
         <v>2157</v>
@@ -2743,13 +2741,13 @@
         <v>2</v>
       </c>
       <c r="D54" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E54">
         <v>5</v>
       </c>
       <c r="F54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G54" s="4">
         <v>1.3540000000000001</v>
@@ -2767,15 +2765,15 @@
         <v>0</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B55">
         <v>2157</v>
@@ -2784,13 +2782,13 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E55">
         <v>6</v>
       </c>
       <c r="F55" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G55" s="4">
         <v>2.8740000000000001</v>
@@ -2808,15 +2806,15 @@
         <v>2.206</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B56">
         <v>2206</v>
@@ -2825,13 +2823,13 @@
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G56" s="4">
         <v>2.5819999999999999</v>
@@ -2849,15 +2847,15 @@
         <v>2.222</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B57">
         <v>2206</v>
@@ -2866,13 +2864,13 @@
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E57">
         <v>2</v>
       </c>
       <c r="F57" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G57" s="4">
         <v>1.883</v>
@@ -2890,15 +2888,15 @@
         <v>0.85399999999999998</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B58">
         <v>2206</v>
@@ -2907,16 +2905,16 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E58">
         <v>3</v>
       </c>
       <c r="F58" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G58" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -2931,15 +2929,15 @@
         <v>0</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B59">
         <v>2206</v>
@@ -2948,16 +2946,16 @@
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E59">
         <v>4</v>
       </c>
       <c r="F59" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G59" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2972,15 +2970,15 @@
         <v>0</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="15" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B60">
         <v>2206</v>
@@ -2989,16 +2987,16 @@
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E60">
         <v>5</v>
       </c>
       <c r="F60" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G60" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -3013,15 +3011,15 @@
         <v>0</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B61">
         <v>2206</v>
@@ -3030,13 +3028,13 @@
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E61">
         <v>6</v>
       </c>
       <c r="F61" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G61" s="4">
         <v>1.33</v>
@@ -3054,15 +3052,15 @@
         <v>0</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:13">
       <c r="A62" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B62">
         <v>2270</v>
@@ -3071,13 +3069,13 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G62" s="4">
         <v>2.202</v>
@@ -3095,15 +3093,15 @@
         <v>0</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:13">
       <c r="A63" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B63">
         <v>2270</v>
@@ -3112,16 +3110,16 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E63">
         <v>2</v>
       </c>
       <c r="F63" t="s">
-        <v>19</v>
-      </c>
-      <c r="G63" s="4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H63">
         <v>2</v>
@@ -3136,15 +3134,15 @@
         <v>0</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="15" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B64">
         <v>2270</v>
@@ -3153,13 +3151,13 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64" t="s">
         <v>20</v>
-      </c>
-      <c r="E64">
-        <v>3</v>
-      </c>
-      <c r="F64" t="s">
-        <v>19</v>
       </c>
       <c r="G64" s="4">
         <v>3.9470000000000001</v>
@@ -3177,15 +3175,15 @@
         <v>0</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="15" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B65">
         <v>2270</v>
@@ -3194,13 +3192,13 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E65">
         <v>4</v>
       </c>
       <c r="F65" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G65" s="4">
         <v>2.2839999999999998</v>
@@ -3218,15 +3216,15 @@
         <v>1.599</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="15" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B66">
         <v>2270</v>
@@ -3235,13 +3233,13 @@
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E66">
         <v>5</v>
       </c>
       <c r="F66" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G66" s="4">
         <v>1.42</v>
@@ -3259,15 +3257,15 @@
         <v>0.29699999999999999</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B67">
         <v>2270</v>
@@ -3276,13 +3274,13 @@
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E67">
         <v>6</v>
       </c>
       <c r="F67" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G67" s="4">
         <v>2.4790000000000001</v>
@@ -3300,15 +3298,15 @@
         <v>1.2649999999999999</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="A68" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B68">
         <v>2272</v>
@@ -3317,16 +3315,16 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E68">
         <v>1</v>
       </c>
       <c r="F68" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -3341,15 +3339,15 @@
         <v>0</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B69">
         <v>2272</v>
@@ -3358,13 +3356,13 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E69">
         <v>2</v>
       </c>
       <c r="F69" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G69" s="4">
         <v>2.5230000000000001</v>
@@ -3382,15 +3380,15 @@
         <v>0</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:13">
       <c r="A70" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B70">
         <v>2272</v>
@@ -3399,16 +3397,16 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E70">
         <v>3</v>
       </c>
       <c r="F70" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G70" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -3423,15 +3421,15 @@
         <v>0</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B71">
         <v>2272</v>
@@ -3440,13 +3438,13 @@
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E71">
         <v>4</v>
       </c>
       <c r="F71" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G71" s="4">
         <v>1.137</v>
@@ -3464,15 +3462,15 @@
         <v>0</v>
       </c>
       <c r="L71" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="A72" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B72">
         <v>2272</v>
@@ -3481,16 +3479,16 @@
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E72">
         <v>5</v>
       </c>
       <c r="F72" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3505,15 +3503,15 @@
         <v>0</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B73">
         <v>2272</v>
@@ -3522,13 +3520,13 @@
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E73">
         <v>6</v>
       </c>
       <c r="F73" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G73" s="4">
         <v>2.9860000000000002</v>
@@ -3546,15 +3544,15 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M73" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B74">
         <v>2169</v>
@@ -3563,13 +3561,13 @@
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E74">
         <v>1</v>
       </c>
       <c r="F74" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G74" s="4">
         <v>1.696</v>
@@ -3587,15 +3585,15 @@
         <v>0</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B75">
         <v>2169</v>
@@ -3604,13 +3602,13 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E75">
         <v>2</v>
       </c>
       <c r="F75" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G75" s="4">
         <v>1.504</v>
@@ -3628,15 +3626,15 @@
         <v>0.50800000000000001</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:13">
       <c r="A76" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B76">
         <v>2169</v>
@@ -3645,16 +3643,16 @@
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E76">
         <v>3</v>
       </c>
       <c r="F76" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -3669,15 +3667,15 @@
         <v>0</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="A77" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B77">
         <v>2169</v>
@@ -3686,16 +3684,16 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E77">
         <v>4</v>
       </c>
       <c r="F77" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -3710,15 +3708,15 @@
         <v>0</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:13">
       <c r="A78" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B78">
         <v>2169</v>
@@ -3727,16 +3725,16 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E78">
         <v>5</v>
       </c>
       <c r="F78" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -3751,15 +3749,15 @@
         <v>0</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:13">
       <c r="A79" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B79">
         <v>2169</v>
@@ -3768,16 +3766,16 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E79">
         <v>6</v>
       </c>
       <c r="F79" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -3792,15 +3790,15 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M79" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:13">
       <c r="A80" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B80">
         <v>1690</v>
@@ -3809,16 +3807,16 @@
         <v>1</v>
       </c>
       <c r="D80" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E80">
         <v>1</v>
       </c>
       <c r="F80" t="s">
-        <v>19</v>
-      </c>
-      <c r="G80" s="4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G80" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H80">
         <v>2</v>
@@ -3833,15 +3831,15 @@
         <v>0</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B81">
         <v>1690</v>
@@ -3850,16 +3848,16 @@
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E81">
         <v>2</v>
       </c>
       <c r="F81" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -3874,15 +3872,15 @@
         <v>0</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:13">
       <c r="A82" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B82">
         <v>1690</v>
@@ -3891,16 +3889,16 @@
         <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E82">
         <v>3</v>
       </c>
       <c r="F82" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -3915,15 +3913,15 @@
         <v>0</v>
       </c>
       <c r="L82" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:13">
       <c r="A83" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B83">
         <v>1690</v>
@@ -3932,16 +3930,16 @@
         <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E83">
         <v>4</v>
       </c>
       <c r="F83" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -3956,15 +3954,15 @@
         <v>0</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:13">
       <c r="A84" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B84">
         <v>1690</v>
@@ -3973,13 +3971,13 @@
         <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E84">
         <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G84" s="4">
         <v>3.5840000000000001</v>
@@ -3997,15 +3995,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="L84" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:13">
       <c r="A85" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B85">
         <v>1690</v>
@@ -4014,13 +4012,13 @@
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E85">
         <v>6</v>
       </c>
       <c r="F85" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G85" s="4">
         <v>1.024</v>
@@ -4038,15 +4036,15 @@
         <v>0</v>
       </c>
       <c r="L85" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M85" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:13">
       <c r="A86" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B86">
         <v>716</v>
@@ -4055,13 +4053,13 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E86">
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G86" s="4">
         <v>1.179</v>
@@ -4079,15 +4077,15 @@
         <v>0</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:13">
       <c r="A87" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B87">
         <v>716</v>
@@ -4096,13 +4094,13 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E87">
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G87" s="4">
         <v>0.89800000000000002</v>
@@ -4120,15 +4118,15 @@
         <v>1.0249999999999999</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:13">
       <c r="A88" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B88">
         <v>716</v>
@@ -4137,13 +4135,13 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E88">
         <v>3</v>
       </c>
       <c r="F88" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G88" s="4">
         <v>1.752</v>
@@ -4161,15 +4159,15 @@
         <v>1.379</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:13">
       <c r="A89" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B89">
         <v>716</v>
@@ -4178,13 +4176,13 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E89">
         <v>4</v>
       </c>
       <c r="F89" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G89" s="4">
         <v>3.3029999999999999</v>
@@ -4202,15 +4200,15 @@
         <v>2.375</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:13">
       <c r="A90" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B90">
         <v>716</v>
@@ -4219,13 +4217,13 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E90">
         <v>5</v>
       </c>
       <c r="F90" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G90" s="4">
         <v>1.7190000000000001</v>
@@ -4243,15 +4241,15 @@
         <v>1.028</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:13">
       <c r="A91" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B91">
         <v>716</v>
@@ -4260,13 +4258,13 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E91">
         <v>6</v>
       </c>
       <c r="F91" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G91" s="4">
         <v>1.7150000000000001</v>
@@ -4284,15 +4282,15 @@
         <v>0</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:13">
       <c r="A92" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B92">
         <v>2334</v>
@@ -4301,13 +4299,13 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E92">
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G92" s="4">
         <v>0.91</v>
@@ -4325,15 +4323,15 @@
         <v>0</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M92" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:13">
       <c r="A93" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B93">
         <v>2334</v>
@@ -4342,16 +4340,16 @@
         <v>3</v>
       </c>
       <c r="D93" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E93">
         <v>2</v>
       </c>
       <c r="F93" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G93" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -4366,15 +4364,15 @@
         <v>0</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:13">
       <c r="A94" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B94">
         <v>2334</v>
@@ -4383,16 +4381,16 @@
         <v>3</v>
       </c>
       <c r="D94" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E94">
         <v>3</v>
       </c>
       <c r="F94" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G94" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -4407,15 +4405,15 @@
         <v>0</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M94" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:13">
       <c r="A95" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B95">
         <v>2334</v>
@@ -4424,13 +4422,13 @@
         <v>3</v>
       </c>
       <c r="D95" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E95">
         <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G95" s="4">
         <v>1.784</v>
@@ -4448,15 +4446,15 @@
         <v>0</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:13">
       <c r="A96" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B96">
         <v>2334</v>
@@ -4465,13 +4463,13 @@
         <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E96">
         <v>5</v>
       </c>
       <c r="F96" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G96" s="4">
         <v>2.133</v>
@@ -4489,15 +4487,15 @@
         <v>0.65700000000000003</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B97">
         <v>2334</v>
@@ -4506,16 +4504,16 @@
         <v>3</v>
       </c>
       <c r="D97" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E97">
         <v>6</v>
       </c>
       <c r="F97" t="s">
-        <v>19</v>
-      </c>
-      <c r="G97" s="4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="G97" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -4530,15 +4528,15 @@
         <v>0</v>
       </c>
       <c r="L97" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M97" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:13">
       <c r="A98" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B98" s="2">
         <v>2275</v>
@@ -4547,16 +4545,16 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E98">
         <v>1</v>
       </c>
       <c r="F98" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G98" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -4571,15 +4569,15 @@
         <v>0</v>
       </c>
       <c r="L98" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:13">
       <c r="A99" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B99">
         <v>2275</v>
@@ -4588,13 +4586,13 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E99">
         <v>2</v>
       </c>
       <c r="F99" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G99" s="4">
         <v>3.2989999999999999</v>
@@ -4612,15 +4610,15 @@
         <v>0.71299999999999997</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M99" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:13">
       <c r="A100" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B100">
         <v>2275</v>
@@ -4629,13 +4627,13 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
+        <v>21</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="F100" t="s">
         <v>20</v>
-      </c>
-      <c r="E100">
-        <v>3</v>
-      </c>
-      <c r="F100" t="s">
-        <v>19</v>
       </c>
       <c r="G100" s="4">
         <v>2.1280000000000001</v>
@@ -4653,15 +4651,15 @@
         <v>0</v>
       </c>
       <c r="L100" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:13">
       <c r="A101" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B101">
         <v>2275</v>
@@ -4670,16 +4668,16 @@
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E101">
         <v>4</v>
       </c>
       <c r="F101" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G101" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -4694,15 +4692,15 @@
         <v>0</v>
       </c>
       <c r="L101" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M101" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B102">
         <v>2275</v>
@@ -4711,13 +4709,13 @@
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E102">
         <v>5</v>
       </c>
       <c r="F102" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G102" s="4">
         <v>5.5</v>
@@ -4735,15 +4733,15 @@
         <v>0.316</v>
       </c>
       <c r="L102" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M102" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:13">
       <c r="A103" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B103">
         <v>2275</v>
@@ -4752,16 +4750,16 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E103">
         <v>6</v>
       </c>
       <c r="F103" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G103" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -4776,10 +4774,10 @@
         <v>0</v>
       </c>
       <c r="L103" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -4848,30 +4846,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>